<commit_message>
Added changes on  Action Plan for Learning
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -1,40 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Trainings\0_Training_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F8BE61-EA89-4A3A-A577-6B53077D6CEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA7420B-A6E7-4660-BF30-8563F24B0D27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="933" firstSheet="1" activeTab="14" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="933" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Career PATH" sheetId="1" r:id="rId1"/>
-    <sheet name="UI Architecture" sheetId="33" r:id="rId2"/>
-    <sheet name="JAVA" sheetId="8" r:id="rId3"/>
-    <sheet name="NODE" sheetId="7" r:id="rId4"/>
-    <sheet name="Python" sheetId="14" r:id="rId5"/>
-    <sheet name="Oracle_Apex" sheetId="15" r:id="rId6"/>
-    <sheet name="Oracle" sheetId="11" r:id="rId7"/>
-    <sheet name="mySQL" sheetId="12" r:id="rId8"/>
-    <sheet name="JavaScript" sheetId="5" r:id="rId9"/>
-    <sheet name="GIT" sheetId="10" r:id="rId10"/>
-    <sheet name="Understanding_DevOps" sheetId="16" r:id="rId11"/>
-    <sheet name="React" sheetId="13" r:id="rId12"/>
-    <sheet name="CSS" sheetId="4" r:id="rId13"/>
-    <sheet name="HTML" sheetId="2" r:id="rId14"/>
-    <sheet name="Angular" sheetId="9" r:id="rId15"/>
-    <sheet name="Sheet1" sheetId="17" r:id="rId16"/>
-    <sheet name="API_Promise" sheetId="18" r:id="rId17"/>
-    <sheet name="API_Promise2" sheetId="19" r:id="rId18"/>
-    <sheet name="API+Observables" sheetId="20" r:id="rId19"/>
+    <sheet name="Career PATH_New" sheetId="35" r:id="rId1"/>
+    <sheet name="Career PATH" sheetId="1" r:id="rId2"/>
+    <sheet name="Professional Scrum" sheetId="34" r:id="rId3"/>
+    <sheet name="Scrum Master" sheetId="33" r:id="rId4"/>
+    <sheet name="JAVA" sheetId="8" r:id="rId5"/>
+    <sheet name="NODE" sheetId="7" r:id="rId6"/>
+    <sheet name="Python" sheetId="14" r:id="rId7"/>
+    <sheet name="Oracle_Apex" sheetId="15" r:id="rId8"/>
+    <sheet name="Oracle" sheetId="11" r:id="rId9"/>
+    <sheet name="mySQL" sheetId="12" r:id="rId10"/>
+    <sheet name="JavaScript" sheetId="5" r:id="rId11"/>
+    <sheet name="GIT" sheetId="10" r:id="rId12"/>
+    <sheet name="Understanding_DevOps" sheetId="16" r:id="rId13"/>
+    <sheet name="React" sheetId="13" r:id="rId14"/>
+    <sheet name="CSS" sheetId="4" r:id="rId15"/>
+    <sheet name="HTML" sheetId="2" r:id="rId16"/>
+    <sheet name="Angular" sheetId="9" r:id="rId17"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId18"/>
+    <sheet name="API_Promise" sheetId="18" r:id="rId19"/>
+    <sheet name="API_Promise2" sheetId="19" r:id="rId20"/>
+    <sheet name="API+Observables" sheetId="20" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Career PATH'!$A$3:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Career PATH'!$A$3:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Career PATH_New'!$A$3:$H$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="208">
   <si>
     <t>SR#</t>
   </si>
@@ -2241,6 +2244,27 @@
   </si>
   <si>
     <t>UI Architecture</t>
+  </si>
+  <si>
+    <t>Scrum Framework</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/paths/skills/the-scrum-framework</t>
+  </si>
+  <si>
+    <t>Scrum Master: https://app.pluralsight.com/paths/skills/the-scrum-framework</t>
+  </si>
+  <si>
+    <t>Introduction to Professional Scrum</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/paths/skills/introduction-to-professional-scrum</t>
+  </si>
+  <si>
+    <t>End to End Testing with Cypress</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/codemash-session-01/table-of-contents</t>
   </si>
 </sst>
 </file>
@@ -2485,7 +2509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2687,6 +2711,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3242,6 +3281,1495 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DD9AF8-082C-4A8A-B3AE-AF46DCC68640}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="39" style="20" customWidth="1"/>
+    <col min="3" max="3" width="67.140625" style="75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>1</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>2</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>3</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>4</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>5</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="45">
+        <v>1</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="64" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="64" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="64" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="24"/>
+      <c r="D23" s="30"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="24"/>
+      <c r="D24" s="30"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="24"/>
+      <c r="D25" s="30"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="24"/>
+      <c r="D26" s="30"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="B29" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="B30" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
+      <c r="B32" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:H20" xr:uid="{D1AE8F92-0427-4F12-8484-D03DDDD5BCBC}"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A27:H27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C18" r:id="rId1" xr:uid="{27A6CB59-A826-4E9D-A404-1E6CC0FFCC9E}"/>
+    <hyperlink ref="C19" r:id="rId2" xr:uid="{D285E2CE-31B5-44B1-A04A-A9152D104B2C}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{1D0A9AAC-FC60-4A0C-BF1B-429F98BFBC13}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{B3EA6DB0-8D3D-4402-B788-E6D11606F0C2}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{07F21C94-E305-46A3-B2BC-1ABCB9139AC5}"/>
+    <hyperlink ref="C17" r:id="rId6" xr:uid="{FA93A347-2A0B-4561-A4F9-54FBC743C313}"/>
+    <hyperlink ref="C15" r:id="rId7" xr:uid="{B09785B5-CC8B-4862-8F5D-7A3BE90945FA}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{1A0CDC41-F082-422E-9D34-1052D7425167}"/>
+    <hyperlink ref="B19" location="HTML!A1" display="HTML" xr:uid="{04F2C601-D41C-41DF-BB28-814D32C67482}"/>
+    <hyperlink ref="C16" r:id="rId9" xr:uid="{1AF4606C-AE95-4BE2-AB1E-1B9033A8B448}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{C98E047B-06C9-4ED4-BA14-8F28A4826EF0}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{724D9E13-D5F3-45AB-A8A6-F626B677F9C6}"/>
+    <hyperlink ref="B6" location="JavaScript!A1" display="JavaScript Path" xr:uid="{570D0166-7D68-4A46-80EC-3B0E13597B03}"/>
+    <hyperlink ref="B18" location="CSS!A1" display="CSS Path" xr:uid="{174ED7E9-2828-460D-85F4-E7B4EB5E0EF1}"/>
+    <hyperlink ref="B8" location="NODE!A1" display="Node Path: Working with Node.js" xr:uid="{934419F1-98EC-4FAC-AEF7-7C3428BD1361}"/>
+    <hyperlink ref="B7" location="JAVA!A1" display="Java Path" xr:uid="{F6C8447A-68BB-4DAE-BA10-12327E641851}"/>
+    <hyperlink ref="B4" location="Angular!A1" display="Angular Path" xr:uid="{807705DC-D889-498E-9FCE-6748242DEDFA}"/>
+    <hyperlink ref="B15" location="GIT!A1" display="GIT Path : Managing Source Code with Git" xr:uid="{78C82B13-55BF-4A2E-912C-4109A844267C}"/>
+    <hyperlink ref="B12" location="Oracle!A1" display="Oracle" xr:uid="{0365AAF3-89CD-4346-A6D6-D2AD6FA60392}"/>
+    <hyperlink ref="B11" location="mySQL!A1" display="mySQL" xr:uid="{FF64FA15-D92F-4640-910B-F0847F18A1F6}"/>
+    <hyperlink ref="B17" location="React!A1" display="React path" xr:uid="{BA7D66AC-FBCD-46A6-832B-20A3EAB22B1B}"/>
+    <hyperlink ref="C9" r:id="rId12" xr:uid="{0AF98188-5C6D-4B95-9B46-7D92E4036190}"/>
+    <hyperlink ref="B9" location="Python!A1" display="Python Path" xr:uid="{9A20957A-ECA8-46D3-9322-58CAECB4DF5F}"/>
+    <hyperlink ref="C10" r:id="rId13" xr:uid="{9BCA941E-4197-452E-9EAD-22D6AD68B17B}"/>
+    <hyperlink ref="B10" location="Oracle_Apex!A1" display="Oracle APEX" xr:uid="{D0058443-A884-45BC-BE4A-674ED0473A57}"/>
+    <hyperlink ref="B16" location="Understanding_DevOps!A1" display="Understanding DevOps [Jenkins CI/CD]" xr:uid="{9ECC36C5-B86D-47BD-8234-8F23DA14849D}"/>
+    <hyperlink ref="C20" r:id="rId14" xr:uid="{A21C8089-CCF6-4DE7-BD38-061FEDB6F4FA}"/>
+    <hyperlink ref="B20" location="'UI Architecture'!A1" display="UI Architecture" xr:uid="{1D90C572-0584-47B2-9682-B1C12A6FA414}"/>
+    <hyperlink ref="C21" r:id="rId15" xr:uid="{EEA7CAD4-5E90-4C59-A71F-B641FB75241C}"/>
+    <hyperlink ref="B21" location="'Scrum Master'!A1" display="Scrum Framework" xr:uid="{46163F81-9396-4C0C-BF39-29A9AE5D0A9A}"/>
+    <hyperlink ref="C22" r:id="rId16" xr:uid="{843DCE90-BFAC-4B3E-8E1E-9285673AAAA5}"/>
+    <hyperlink ref="B22" location="'Professional Scrum'!A1" display="Introduction to Professional Scrum" xr:uid="{3414B9DA-2364-4D11-9DD8-7459D1C5FC58}"/>
+    <hyperlink ref="C5" r:id="rId17" xr:uid="{07035312-F938-47F5-9C1B-09FD16F8785D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6538CA4A-D841-48B5-87FD-DBB4645DC6A3}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{E24D082F-65BA-4F5C-BAB7-0599305D0FF8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA157C68-6EB3-4779-91CE-4005608DD947}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{FEB0B8AC-E899-4404-99C4-C73641227134}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27645D63-80B6-4CC9-9DF9-3EC673CAFE41}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{98A3AB38-E903-4B3C-88B3-6A5C5BC702D7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9B2914-37AB-487B-B6E7-416C38CF27C7}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{09ECF932-C23A-44CD-8179-FF32CD837195}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148D65EB-A89E-42AB-9829-0D129960DFD3}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{4BA727F5-8C8F-464B-91D2-FD6D9F2A896F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC9DC54-2F87-41CA-B048-C3AF3C22C7C1}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{7C4ABC16-6947-4C5D-ABBE-56F581C7C54B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371B9012-BBC9-4C0D-A9EB-8BF65ACEAE9A}">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="40"/>
+    <col min="2" max="3" width="19.140625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" style="35" customWidth="1"/>
+    <col min="5" max="5" width="65.42578125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="28" style="35" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="35" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40">
+        <v>1</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
+        <v>2</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="D9" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="D12" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="D13" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="D14" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="D15" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C16" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="D18" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="C19" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C22" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="D23" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D24" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C25" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D26" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="D27" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="C28" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="E29" s="36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="E30" s="36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="E31" s="36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D32" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" s="36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{A0B3118C-57C0-462F-9A14-B28973E6A144}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A0C1A6-B2EA-4EC5-8484-E684C8F3E18B}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="59"/>
+    <col min="2" max="2" width="41.42578125" style="63" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="63" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" style="62" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="55" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="55" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="55"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="54"/>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="59">
+        <v>1</v>
+      </c>
+      <c r="B3" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="60" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="55"/>
+      <c r="B4" s="61" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="61" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="52"/>
+    </row>
+    <row r="6" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="B6" s="61"/>
+      <c r="C6" s="61" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="61"/>
+      <c r="C7" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D8" s="62" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="D9" s="62" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="D10" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="52" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="D11" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="60" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="B13" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="D14" s="62" t="s">
+        <v>173</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D15" s="62" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="C16" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="62" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" s="55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D18" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="D19" s="62" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="62" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="D20" s="62" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" s="52" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="D21" s="62" t="s">
+        <v>190</v>
+      </c>
+      <c r="E21" s="52" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="D22" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="52" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="E23" s="52" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="62" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="C25" s="62" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="62" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{48B2311E-C92A-45B3-8C52-8F1CD3A62F14}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E0624A-E488-4F43-A83F-9652CAB5AAD3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C00811-F6B3-4257-85C9-1B55DCD46308}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DB7C02-07A8-4D5B-B7A9-996091B89DD9}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -3249,7 +4777,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3484,13 +5012,27 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
-      <c r="B18" s="24"/>
-      <c r="D18" s="30"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="64" t="s">
+        <v>201</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
-      <c r="B19" s="24"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="64" t="s">
+        <v>204</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
@@ -3620,924 +5162,17 @@
     <hyperlink ref="B13" location="Understanding_DevOps!A1" display="Understanding DevOps [Jenkins CI/CD]" xr:uid="{4DD60EA1-7E35-4161-8A6E-382DD256E589}"/>
     <hyperlink ref="C17" r:id="rId14" xr:uid="{D2A3E277-9FE0-48D8-BA95-827DBC236E38}"/>
     <hyperlink ref="B17" location="'UI Architecture'!A1" display="UI Architecture" xr:uid="{7240D223-15FC-45EE-9E3A-9B8908130345}"/>
+    <hyperlink ref="C18" r:id="rId15" xr:uid="{095E8D3B-1363-488A-8B7C-617A45686604}"/>
+    <hyperlink ref="B18" location="'Scrum Master'!A1" display="Scrum Framework" xr:uid="{886D537C-A45A-404C-BB05-10F0E27873C1}"/>
+    <hyperlink ref="C19" r:id="rId16" xr:uid="{2310128F-5B6E-4D76-916B-4F9216A64190}"/>
+    <hyperlink ref="B19" location="'Professional Scrum'!A1" display="Introduction to Professional Scrum" xr:uid="{B412A61E-A6A3-430D-8A36-914377A0A709}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27645D63-80B6-4CC9-9DF9-3EC673CAFE41}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{98A3AB38-E903-4B3C-88B3-6A5C5BC702D7}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9B2914-37AB-487B-B6E7-416C38CF27C7}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{09ECF932-C23A-44CD-8179-FF32CD837195}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148D65EB-A89E-42AB-9829-0D129960DFD3}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{4BA727F5-8C8F-464B-91D2-FD6D9F2A896F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC9DC54-2F87-41CA-B048-C3AF3C22C7C1}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{7C4ABC16-6947-4C5D-ABBE-56F581C7C54B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371B9012-BBC9-4C0D-A9EB-8BF65ACEAE9A}">
-  <dimension ref="A1:G32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="40"/>
-    <col min="2" max="3" width="19.140625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="41.42578125" style="35" customWidth="1"/>
-    <col min="5" max="5" width="65.42578125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="28" style="35" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="35" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="35"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40">
-        <v>1</v>
-      </c>
-      <c r="B3" s="69" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D5" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="40">
-        <v>2</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="D9" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D11" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="D12" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="D13" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="D14" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="D15" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C16" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="D18" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="C19" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="50" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="D21" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C22" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="D23" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="36" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="D24" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" s="36" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C25" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="D26" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="36" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="D27" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="36" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="C28" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="36" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="E29" s="36" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="E30" s="36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="E31" s="36" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="D32" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="E32" s="36" t="s">
-        <v>147</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{A0B3118C-57C0-462F-9A14-B28973E6A144}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A0C1A6-B2EA-4EC5-8484-E684C8F3E18B}">
-  <dimension ref="A1:G25"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="59"/>
-    <col min="2" max="2" width="41.42578125" style="63" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="63" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" style="62" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" style="55" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="55" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="55"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="54"/>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="59">
-        <v>1</v>
-      </c>
-      <c r="B3" s="70" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="60" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
-      <c r="B4" s="61" t="s">
-        <v>155</v>
-      </c>
-      <c r="C4" s="61" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="61" t="s">
-        <v>156</v>
-      </c>
-      <c r="C5" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="62" t="s">
-        <v>159</v>
-      </c>
-      <c r="E5" s="52"/>
-    </row>
-    <row r="6" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="B6" s="61"/>
-      <c r="C6" s="61" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="62" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="61"/>
-      <c r="C7" s="61" t="s">
-        <v>161</v>
-      </c>
-      <c r="D7" s="62" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D8" s="62" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="D9" s="62" t="s">
-        <v>184</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="D10" s="62" t="s">
-        <v>185</v>
-      </c>
-      <c r="E10" s="52" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="D11" s="62" t="s">
-        <v>166</v>
-      </c>
-      <c r="E11" s="52" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="70" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="60" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="B13" s="63" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="63" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="E13" s="52" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="D14" s="62" t="s">
-        <v>173</v>
-      </c>
-      <c r="E14" s="52" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D15" s="62" t="s">
-        <v>175</v>
-      </c>
-      <c r="E15" s="52" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="C16" s="63" t="s">
-        <v>168</v>
-      </c>
-      <c r="D16" s="62" t="s">
-        <v>177</v>
-      </c>
-      <c r="E16" s="62" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="62" t="s">
-        <v>179</v>
-      </c>
-      <c r="E17" s="55" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="D18" s="62" t="s">
-        <v>181</v>
-      </c>
-      <c r="E18" s="52" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="D19" s="62" t="s">
-        <v>186</v>
-      </c>
-      <c r="E19" s="62" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="D20" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="E20" s="52" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="D21" s="62" t="s">
-        <v>190</v>
-      </c>
-      <c r="E21" s="52" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="D22" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" s="52" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="E23" s="52" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="62" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="C25" s="62" t="s">
-        <v>196</v>
-      </c>
-      <c r="D25" s="62" t="s">
-        <v>198</v>
-      </c>
-      <c r="E25" s="52" t="s">
-        <v>197</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{48B2311E-C92A-45B3-8C52-8F1CD3A62F14}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E0624A-E488-4F43-A83F-9652CAB5AAD3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C00811-F6B3-4257-85C9-1B55DCD46308}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3239CF-6342-4294-A04F-B9BB3AB32E10}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4551,7 +5186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCADFB6-2B39-4345-B261-07B732A46DA7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4567,24 +5202,147 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8600B75A-1ED1-437D-9B1E-4EB6353449BE}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4382FB-CCDB-4DE4-9683-3A8D07D3F404}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{506261BB-1887-4269-878D-19C280DF4387}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8600B75A-1ED1-437D-9B1E-4EB6353449BE}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{CB8EDE69-F642-47A0-955A-62F71D60EEEB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA77D0AC-A7B6-4319-A90C-CAC41021F832}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4650,7 +5408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F09BD98-79D8-450C-972D-16EC9C4FC717}">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -4799,7 +5557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBA4A8B-062F-4280-B637-4D3543B7B63A}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -4869,7 +5627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC297CD3-0B1F-4BB7-8CC6-619A9FF0CD07}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -4939,7 +5697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FCCAF4-6438-4808-B747-7037D39019AA}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -5003,146 +5761,6 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{8DEDA224-60F6-4096-98B1-F0878FA4FCE6}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6538CA4A-D841-48B5-87FD-DBB4645DC6A3}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{E24D082F-65BA-4F5C-BAB7-0599305D0FF8}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA157C68-6EB3-4779-91CE-4005608DD947}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{FEB0B8AC-E899-4404-99C4-C73641227134}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Developer to Architect file
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Trainings\0_Training_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA7420B-A6E7-4660-BF30-8563F24B0D27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687B2AFC-B395-4013-A59E-152667407863}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="933" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Career PATH_New" sheetId="35" r:id="rId1"/>
+    <sheet name="Career PATH_Improved" sheetId="35" r:id="rId1"/>
     <sheet name="Career PATH" sheetId="1" r:id="rId2"/>
     <sheet name="Professional Scrum" sheetId="34" r:id="rId3"/>
     <sheet name="Scrum Master" sheetId="33" r:id="rId4"/>
@@ -37,7 +37,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Career PATH'!$A$3:$H$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Career PATH_New'!$A$3:$H$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Career PATH_Improved'!$A$3:$H$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="217">
   <si>
     <t>SR#</t>
   </si>
@@ -2265,6 +2265,36 @@
   </si>
   <si>
     <t>https://app.pluralsight.com/library/courses/codemash-session-01/table-of-contents</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/cypress-end-to-end-javascript-testing/recommended-courses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Cypress: End-to-end JavaScript Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Automated Testing All the Things with Cypress</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/js-friends-session-02/table-of-contents</t>
+  </si>
+  <si>
+    <t>Automated Testing: End to End</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/automated-testing-end-to-end/table-of-contents</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/developer-to-architect/table-of-contents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Developer to Architect</t>
+  </si>
+  <si>
+    <t>https://codedamn.com/learning-paths/fullstack</t>
   </si>
 </sst>
 </file>
@@ -2425,7 +2455,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2480,6 +2510,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2509,7 +2545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2691,6 +2727,30 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2711,21 +2771,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3285,17 +3330,17 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="39" style="20" customWidth="1"/>
-    <col min="3" max="3" width="67.140625" style="75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.140625" style="68" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
@@ -3304,35 +3349,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="66" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -3364,10 +3409,10 @@
       <c r="D4" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
@@ -3382,339 +3427,403 @@
       <c r="D5" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
-        <v>3</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="74" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
-        <v>4</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>17</v>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="70" t="s">
+        <v>212</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="74" t="s">
-        <v>52</v>
+        <v>213</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>214</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <v>5</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>56</v>
+      <c r="E9" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>3</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>9</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>39</v>
       </c>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>4</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>5</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D15" s="28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="22" t="s">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C16" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D16" s="28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="22" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C19" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D19" s="29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="23" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C20" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D20" s="29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="22" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C21" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D21" s="29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="33" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C22" s="67" t="s">
         <v>8</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="45">
-        <v>1</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="64" t="s">
-        <v>200</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="64" t="s">
-        <v>201</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="64" t="s">
-        <v>204</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>205</v>
       </c>
       <c r="D22" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="24"/>
-      <c r="D23" s="30"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="45">
+        <v>1</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="24"/>
-      <c r="D24" s="30"/>
+      <c r="B24" s="64" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
-      <c r="B25" s="24"/>
-      <c r="D25" s="30"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="64" t="s">
+        <v>201</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
-      <c r="B26" s="24"/>
-      <c r="D26" s="30"/>
+      <c r="B26" s="64" t="s">
+        <v>204</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="24"/>
+      <c r="D27" s="30"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="76" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" t="s">
-        <v>37</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="A28" s="15"/>
+      <c r="B28" s="24"/>
+      <c r="D28" s="30"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
-      <c r="B29" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="76" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B29" s="24"/>
+      <c r="D29" s="30"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A30" s="15"/>
+      <c r="B30" s="24"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A31" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+      <c r="B34" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
+      <c r="B36" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:H20" xr:uid="{D1AE8F92-0427-4F12-8484-D03DDDD5BCBC}"/>
+  <autoFilter ref="A3:H24" xr:uid="{D1AE8F92-0427-4F12-8484-D03DDDD5BCBC}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A31:H31"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C18" r:id="rId1" xr:uid="{27A6CB59-A826-4E9D-A404-1E6CC0FFCC9E}"/>
-    <hyperlink ref="C19" r:id="rId2" xr:uid="{D285E2CE-31B5-44B1-A04A-A9152D104B2C}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{1D0A9AAC-FC60-4A0C-BF1B-429F98BFBC13}"/>
+    <hyperlink ref="C22" r:id="rId1" xr:uid="{27A6CB59-A826-4E9D-A404-1E6CC0FFCC9E}"/>
+    <hyperlink ref="C23" r:id="rId2" xr:uid="{D285E2CE-31B5-44B1-A04A-A9152D104B2C}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{1D0A9AAC-FC60-4A0C-BF1B-429F98BFBC13}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{B3EA6DB0-8D3D-4402-B788-E6D11606F0C2}"/>
-    <hyperlink ref="C7" r:id="rId5" xr:uid="{07F21C94-E305-46A3-B2BC-1ABCB9139AC5}"/>
-    <hyperlink ref="C17" r:id="rId6" xr:uid="{FA93A347-2A0B-4561-A4F9-54FBC743C313}"/>
-    <hyperlink ref="C15" r:id="rId7" xr:uid="{B09785B5-CC8B-4862-8F5D-7A3BE90945FA}"/>
-    <hyperlink ref="C8" r:id="rId8" xr:uid="{1A0CDC41-F082-422E-9D34-1052D7425167}"/>
-    <hyperlink ref="B19" location="HTML!A1" display="HTML" xr:uid="{04F2C601-D41C-41DF-BB28-814D32C67482}"/>
-    <hyperlink ref="C16" r:id="rId9" xr:uid="{1AF4606C-AE95-4BE2-AB1E-1B9033A8B448}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{C98E047B-06C9-4ED4-BA14-8F28A4826EF0}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{724D9E13-D5F3-45AB-A8A6-F626B677F9C6}"/>
-    <hyperlink ref="B6" location="JavaScript!A1" display="JavaScript Path" xr:uid="{570D0166-7D68-4A46-80EC-3B0E13597B03}"/>
-    <hyperlink ref="B18" location="CSS!A1" display="CSS Path" xr:uid="{174ED7E9-2828-460D-85F4-E7B4EB5E0EF1}"/>
-    <hyperlink ref="B8" location="NODE!A1" display="Node Path: Working with Node.js" xr:uid="{934419F1-98EC-4FAC-AEF7-7C3428BD1361}"/>
-    <hyperlink ref="B7" location="JAVA!A1" display="Java Path" xr:uid="{F6C8447A-68BB-4DAE-BA10-12327E641851}"/>
+    <hyperlink ref="C11" r:id="rId5" xr:uid="{07F21C94-E305-46A3-B2BC-1ABCB9139AC5}"/>
+    <hyperlink ref="C21" r:id="rId6" xr:uid="{FA93A347-2A0B-4561-A4F9-54FBC743C313}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{B09785B5-CC8B-4862-8F5D-7A3BE90945FA}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{1A0CDC41-F082-422E-9D34-1052D7425167}"/>
+    <hyperlink ref="B23" location="HTML!A1" display="HTML" xr:uid="{04F2C601-D41C-41DF-BB28-814D32C67482}"/>
+    <hyperlink ref="C20" r:id="rId9" xr:uid="{1AF4606C-AE95-4BE2-AB1E-1B9033A8B448}"/>
+    <hyperlink ref="C15" r:id="rId10" xr:uid="{C98E047B-06C9-4ED4-BA14-8F28A4826EF0}"/>
+    <hyperlink ref="C16" r:id="rId11" xr:uid="{724D9E13-D5F3-45AB-A8A6-F626B677F9C6}"/>
+    <hyperlink ref="B10" location="JavaScript!A1" display="JavaScript Path" xr:uid="{570D0166-7D68-4A46-80EC-3B0E13597B03}"/>
+    <hyperlink ref="B22" location="CSS!A1" display="CSS Path" xr:uid="{174ED7E9-2828-460D-85F4-E7B4EB5E0EF1}"/>
+    <hyperlink ref="B12" location="NODE!A1" display="Node Path: Working with Node.js" xr:uid="{934419F1-98EC-4FAC-AEF7-7C3428BD1361}"/>
+    <hyperlink ref="B11" location="JAVA!A1" display="Java Path" xr:uid="{F6C8447A-68BB-4DAE-BA10-12327E641851}"/>
     <hyperlink ref="B4" location="Angular!A1" display="Angular Path" xr:uid="{807705DC-D889-498E-9FCE-6748242DEDFA}"/>
-    <hyperlink ref="B15" location="GIT!A1" display="GIT Path : Managing Source Code with Git" xr:uid="{78C82B13-55BF-4A2E-912C-4109A844267C}"/>
-    <hyperlink ref="B12" location="Oracle!A1" display="Oracle" xr:uid="{0365AAF3-89CD-4346-A6D6-D2AD6FA60392}"/>
-    <hyperlink ref="B11" location="mySQL!A1" display="mySQL" xr:uid="{FF64FA15-D92F-4640-910B-F0847F18A1F6}"/>
-    <hyperlink ref="B17" location="React!A1" display="React path" xr:uid="{BA7D66AC-FBCD-46A6-832B-20A3EAB22B1B}"/>
-    <hyperlink ref="C9" r:id="rId12" xr:uid="{0AF98188-5C6D-4B95-9B46-7D92E4036190}"/>
-    <hyperlink ref="B9" location="Python!A1" display="Python Path" xr:uid="{9A20957A-ECA8-46D3-9322-58CAECB4DF5F}"/>
-    <hyperlink ref="C10" r:id="rId13" xr:uid="{9BCA941E-4197-452E-9EAD-22D6AD68B17B}"/>
-    <hyperlink ref="B10" location="Oracle_Apex!A1" display="Oracle APEX" xr:uid="{D0058443-A884-45BC-BE4A-674ED0473A57}"/>
-    <hyperlink ref="B16" location="Understanding_DevOps!A1" display="Understanding DevOps [Jenkins CI/CD]" xr:uid="{9ECC36C5-B86D-47BD-8234-8F23DA14849D}"/>
-    <hyperlink ref="C20" r:id="rId14" xr:uid="{A21C8089-CCF6-4DE7-BD38-061FEDB6F4FA}"/>
-    <hyperlink ref="B20" location="'UI Architecture'!A1" display="UI Architecture" xr:uid="{1D90C572-0584-47B2-9682-B1C12A6FA414}"/>
-    <hyperlink ref="C21" r:id="rId15" xr:uid="{EEA7CAD4-5E90-4C59-A71F-B641FB75241C}"/>
-    <hyperlink ref="B21" location="'Scrum Master'!A1" display="Scrum Framework" xr:uid="{46163F81-9396-4C0C-BF39-29A9AE5D0A9A}"/>
-    <hyperlink ref="C22" r:id="rId16" xr:uid="{843DCE90-BFAC-4B3E-8E1E-9285673AAAA5}"/>
-    <hyperlink ref="B22" location="'Professional Scrum'!A1" display="Introduction to Professional Scrum" xr:uid="{3414B9DA-2364-4D11-9DD8-7459D1C5FC58}"/>
+    <hyperlink ref="B19" location="GIT!A1" display="GIT Path : Managing Source Code with Git" xr:uid="{78C82B13-55BF-4A2E-912C-4109A844267C}"/>
+    <hyperlink ref="B16" location="Oracle!A1" display="Oracle" xr:uid="{0365AAF3-89CD-4346-A6D6-D2AD6FA60392}"/>
+    <hyperlink ref="B15" location="mySQL!A1" display="mySQL" xr:uid="{FF64FA15-D92F-4640-910B-F0847F18A1F6}"/>
+    <hyperlink ref="B21" location="React!A1" display="React path" xr:uid="{BA7D66AC-FBCD-46A6-832B-20A3EAB22B1B}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{0AF98188-5C6D-4B95-9B46-7D92E4036190}"/>
+    <hyperlink ref="B13" location="Python!A1" display="Python Path" xr:uid="{9A20957A-ECA8-46D3-9322-58CAECB4DF5F}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{9BCA941E-4197-452E-9EAD-22D6AD68B17B}"/>
+    <hyperlink ref="B14" location="Oracle_Apex!A1" display="Oracle APEX" xr:uid="{D0058443-A884-45BC-BE4A-674ED0473A57}"/>
+    <hyperlink ref="B20" location="Understanding_DevOps!A1" display="Understanding DevOps [Jenkins CI/CD]" xr:uid="{9ECC36C5-B86D-47BD-8234-8F23DA14849D}"/>
+    <hyperlink ref="C24" r:id="rId14" xr:uid="{A21C8089-CCF6-4DE7-BD38-061FEDB6F4FA}"/>
+    <hyperlink ref="B24" location="'UI Architecture'!A1" display="UI Architecture" xr:uid="{1D90C572-0584-47B2-9682-B1C12A6FA414}"/>
+    <hyperlink ref="C25" r:id="rId15" xr:uid="{EEA7CAD4-5E90-4C59-A71F-B641FB75241C}"/>
+    <hyperlink ref="B25" location="'Scrum Master'!A1" display="Scrum Framework" xr:uid="{46163F81-9396-4C0C-BF39-29A9AE5D0A9A}"/>
+    <hyperlink ref="C26" r:id="rId16" xr:uid="{843DCE90-BFAC-4B3E-8E1E-9285673AAAA5}"/>
+    <hyperlink ref="B26" location="'Professional Scrum'!A1" display="Introduction to Professional Scrum" xr:uid="{3414B9DA-2364-4D11-9DD8-7459D1C5FC58}"/>
     <hyperlink ref="C5" r:id="rId17" xr:uid="{07035312-F938-47F5-9C1B-09FD16F8785D}"/>
+    <hyperlink ref="C6" r:id="rId18" xr:uid="{B618894D-13D8-4D74-AC21-E78B1007251C}"/>
+    <hyperlink ref="C7" r:id="rId19" xr:uid="{6ABE18E5-17E3-43E0-9C21-2A8D6A7E85FB}"/>
+    <hyperlink ref="C8" r:id="rId20" xr:uid="{B9E5E285-66D9-4C08-BA1E-C21A37C23BD7}"/>
+    <hyperlink ref="E9" r:id="rId21" xr:uid="{B61A0FBF-0638-4233-90E0-B1D44DE7D1B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -3739,14 +3848,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3809,14 +3918,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3881,14 +3990,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3951,14 +4060,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4021,14 +4130,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4091,14 +4200,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4162,12 +4271,12 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
     </row>
@@ -4194,11 +4303,11 @@
       <c r="A3" s="40">
         <v>1</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="77" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
       <c r="E3" s="51" t="s">
         <v>150</v>
       </c>
@@ -4494,12 +4603,12 @@
       <c r="A1" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
       <c r="F1" s="54"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4525,11 +4634,11 @@
       <c r="A3" s="59">
         <v>1</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="78" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
       <c r="E3" s="60" t="s">
         <v>151</v>
       </c>
@@ -4606,11 +4715,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="60" t="s">
         <v>151</v>
       </c>
@@ -4793,28 +4902,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -5055,16 +5164,16 @@
       <c r="D23" s="30"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
@@ -5220,14 +5329,14 @@
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5287,14 +5396,14 @@
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5359,14 +5468,14 @@
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5429,13 +5538,13 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
       <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -5578,14 +5687,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5648,14 +5757,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5718,14 +5827,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Added new changes in 1_developer to architect.docx
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Trainings\0_Training_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFC18F0-7F1D-4CD1-8287-870833B58886}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67399C4D-9211-4E79-9EB5-AA8213A82AE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="933" activeTab="2" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="933" activeTab="2" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Career PATH_Improved" sheetId="35" r:id="rId1"/>
@@ -5671,7 +5671,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new changes with new file
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Trainings\0_Training_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACEF22F-9D13-4B78-A093-CF58B5B64A33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4BAAE5-5DD5-40B3-8375-AD0EDD26F9E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="933" activeTab="3" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="476">
   <si>
     <t>SR#</t>
   </si>
@@ -7990,9 +7990,6 @@
       </rPr>
       <t>?</t>
     </r>
-  </si>
-  <si>
-    <t>`</t>
   </si>
 </sst>
 </file>
@@ -20027,67 +20024,6 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>674</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>674</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="205" name="Picture 204">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4887A6DA-9B1B-4A47-89FE-5F01F179609B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="129797175"/>
-          <a:ext cx="152400" cy="152400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>679</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -20178,67 +20114,6 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>681</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>681</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="208" name="Picture 207">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46F04A70-14CD-424F-B88D-5427D01E94DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="131140200"/>
-          <a:ext cx="152400" cy="152400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
@@ -23189,8 +23064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA30601C-745F-4897-9A38-C5CE8E1BD080}">
   <dimension ref="A1:A689"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A677" workbookViewId="0">
-      <selection activeCell="A678" sqref="A678:A683"/>
+    <sheetView tabSelected="1" topLeftCell="A668" workbookViewId="0">
+      <selection activeCell="A670" sqref="A670"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26099,17 +25974,13 @@
       <c r="A671" s="128"/>
     </row>
     <row r="672" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A672" s="129" t="s">
-        <v>245</v>
-      </c>
+      <c r="A672" s="129"/>
     </row>
     <row r="673" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A673" s="129"/>
     </row>
     <row r="674" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A674" s="129" t="s">
-        <v>367</v>
-      </c>
+      <c r="A674" s="129"/>
     </row>
     <row r="675" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A675" s="129"/>
@@ -26125,30 +25996,22 @@
       </c>
     </row>
     <row r="678" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A678" s="128" t="s">
-        <v>476</v>
-      </c>
+      <c r="A678" s="128"/>
     </row>
     <row r="679" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A679" s="129" t="s">
-        <v>245</v>
-      </c>
+      <c r="A679" s="129"/>
     </row>
     <row r="680" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A680" s="129"/>
     </row>
     <row r="681" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A681" s="129" t="s">
-        <v>367</v>
-      </c>
+      <c r="A681" s="129"/>
     </row>
     <row r="682" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A682" s="129"/>
     </row>
     <row r="683" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A683" s="126" t="s">
-        <v>260</v>
-      </c>
+      <c r="A683" s="126"/>
     </row>
     <row r="684" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A684" s="127" t="s">
@@ -26159,17 +26022,13 @@
       <c r="A685" s="128"/>
     </row>
     <row r="686" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A686" s="129" t="s">
-        <v>245</v>
-      </c>
+      <c r="A686" s="129"/>
     </row>
     <row r="687" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A687" s="129"/>
     </row>
     <row r="688" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A688" s="129" t="s">
-        <v>425</v>
-      </c>
+      <c r="A688" s="129"/>
     </row>
     <row r="689" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A689" s="129"/>

</xml_diff>

<commit_message>
Timesheet Updated for Cypress assignment
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -8,38 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Trainings\0_Training_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BF7951-1BDC-4D5D-AE48-77A73BE26164}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC3F2A7-C8CA-4D83-8CA3-33748E36B6B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="933" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Track_Hours_For_Cypress" sheetId="37" r:id="rId1"/>
-    <sheet name="Career PATH_Improved" sheetId="35" r:id="rId2"/>
-    <sheet name="Career PATH" sheetId="1" r:id="rId3"/>
-    <sheet name="Developer to Architect" sheetId="34" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="36" r:id="rId5"/>
-    <sheet name="Scrum Master" sheetId="33" r:id="rId6"/>
-    <sheet name="JAVA" sheetId="8" r:id="rId7"/>
-    <sheet name="NODE" sheetId="7" r:id="rId8"/>
-    <sheet name="Python" sheetId="14" r:id="rId9"/>
-    <sheet name="Oracle_Apex" sheetId="15" r:id="rId10"/>
-    <sheet name="Oracle" sheetId="11" r:id="rId11"/>
-    <sheet name="mySQL" sheetId="12" r:id="rId12"/>
-    <sheet name="JavaScript" sheetId="5" r:id="rId13"/>
-    <sheet name="GIT" sheetId="10" r:id="rId14"/>
-    <sheet name="Understanding_DevOps" sheetId="16" r:id="rId15"/>
-    <sheet name="React" sheetId="13" r:id="rId16"/>
-    <sheet name="CSS" sheetId="4" r:id="rId17"/>
-    <sheet name="HTML" sheetId="2" r:id="rId18"/>
-    <sheet name="Angular" sheetId="9" r:id="rId19"/>
-    <sheet name="Sheet1" sheetId="17" r:id="rId20"/>
-    <sheet name="API_Promise" sheetId="18" r:id="rId21"/>
-    <sheet name="API_Promise2" sheetId="19" r:id="rId22"/>
-    <sheet name="API+Observables" sheetId="20" r:id="rId23"/>
+    <sheet name="Career PATH_Interactive" sheetId="38" r:id="rId2"/>
+    <sheet name="Career PATH_Improved" sheetId="35" r:id="rId3"/>
+    <sheet name="Career PATH" sheetId="1" r:id="rId4"/>
+    <sheet name="Developer to Architect" sheetId="34" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="36" r:id="rId6"/>
+    <sheet name="Scrum Master" sheetId="33" r:id="rId7"/>
+    <sheet name="JAVA" sheetId="8" r:id="rId8"/>
+    <sheet name="NODE" sheetId="7" r:id="rId9"/>
+    <sheet name="Python" sheetId="14" r:id="rId10"/>
+    <sheet name="Oracle_Apex" sheetId="15" r:id="rId11"/>
+    <sheet name="Oracle" sheetId="11" r:id="rId12"/>
+    <sheet name="mySQL" sheetId="12" r:id="rId13"/>
+    <sheet name="JavaScript" sheetId="5" r:id="rId14"/>
+    <sheet name="GIT" sheetId="10" r:id="rId15"/>
+    <sheet name="Understanding_DevOps" sheetId="16" r:id="rId16"/>
+    <sheet name="React" sheetId="13" r:id="rId17"/>
+    <sheet name="CSS" sheetId="4" r:id="rId18"/>
+    <sheet name="HTML" sheetId="2" r:id="rId19"/>
+    <sheet name="Angular" sheetId="9" r:id="rId20"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId21"/>
+    <sheet name="API_Promise" sheetId="18" r:id="rId22"/>
+    <sheet name="API_Promise2" sheetId="19" r:id="rId23"/>
+    <sheet name="API+Observables" sheetId="20" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Career PATH'!$A$3:$H$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Career PATH_Improved'!$A$3:$F$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Career PATH'!$A$3:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Career PATH_Improved'!$A$3:$F$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Career PATH_Interactive'!$A$3:$F$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="528">
   <si>
     <t>SR#</t>
   </si>
@@ -8070,7 +8072,175 @@
     <t>7.35pm - 9.55pm</t>
   </si>
   <si>
-    <t>7.05am - 9.05</t>
+    <t>RXJS: Getting Started with Reactive Programming Using RxJS</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/reactive-programming-rxjs-getting-started/table-of-contents</t>
+  </si>
+  <si>
+    <t>RxJS: Getting Started</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/rxjs-getting-started/table-of-contents</t>
+  </si>
+  <si>
+    <t>RxJS: The Big Picture</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/rxjs-big-picture/table-of-contents</t>
+  </si>
+  <si>
+    <t>RxJS: Asynchronous Programming in JavaScript (with Rx.js Observables)</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/asynchronous-javascript-rxjs-observables/table-of-contents</t>
+  </si>
+  <si>
+    <t>Learning RxJS: Operators by Example Playbook</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/rxjs-operators-by-example-playbook/table-of-contents</t>
+  </si>
+  <si>
+    <t>Workshop: Advanced RxJS Part 1</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/ng-conf-2021-session-37-part-1/table-of-contents</t>
+  </si>
+  <si>
+    <t>Redux: Redux Fundamentals</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/redux-fundamentals/table-of-contents</t>
+  </si>
+  <si>
+    <t>Cypress: End-to-end JavaScript Testing</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/cypress-end-to-end-javascript-testing/table-of-contents?aid=7010a000002BWq6AAG</t>
+  </si>
+  <si>
+    <t>https://www.learnrxjs.io/</t>
+  </si>
+  <si>
+    <t>RxJS Artifacts</t>
+  </si>
+  <si>
+    <t>RxJS Learning</t>
+  </si>
+  <si>
+    <t>RxJS Play Ground</t>
+  </si>
+  <si>
+    <t>https://rxjs-playground.github.io/#/</t>
+  </si>
+  <si>
+    <t>Fake REST APIS</t>
+  </si>
+  <si>
+    <t>npm install -g json-sever</t>
+  </si>
+  <si>
+    <t>Angular - Kud</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Angular 2</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://www.youtube.com/watch?v=C8JcGqQdcPI
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Creating angular 6 project</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://www.youtube.com/watch?v=CusfUmB6mkY&amp;list=PL6n9fhu94yhWNJaDgh0mfae_9xoQ4E_Zj
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Angular CLI</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://www.youtube.com/watch?v=rJ9o4TyhSuo&amp;list=PL6n9fhu94yhWUcq5Pc16uf8YKXoZ87Vh_
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Angular CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://www.youtube.com/watch?v=JYPyy-hvjYc&amp;list=PL6n9fhu94yhXwcl3a6rIfAI7QmGYIkfK5</t>
+    </r>
+  </si>
+  <si>
+    <t>7.02am - 9.30am</t>
+  </si>
+  <si>
+    <t>7.05am - 9.05am</t>
   </si>
 </sst>
 </file>
@@ -8518,7 +8688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8911,17 +9081,77 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8933,6 +9163,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -20933,7 +21169,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20947,14 +21183,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="164" t="s">
         <v>494</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="164"/>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="120" t="s">
@@ -21323,7 +21559,7 @@
         <v>44558</v>
       </c>
       <c r="D20" t="s">
-        <v>501</v>
+        <v>527</v>
       </c>
       <c r="E20" s="5">
         <v>2</v>
@@ -21342,6 +21578,12 @@
       <c r="C21" s="119">
         <v>44559</v>
       </c>
+      <c r="D21" t="s">
+        <v>526</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2.2799999999999998</v>
+      </c>
       <c r="F21" s="5">
         <v>2</v>
       </c>
@@ -21545,13 +21787,13 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="143" t="s">
+      <c r="C35" s="165" t="s">
         <v>491</v>
       </c>
-      <c r="D35" s="143"/>
+      <c r="D35" s="165"/>
       <c r="E35" s="126">
         <f>SUM(E3:E34)</f>
-        <v>29.11</v>
+        <v>31.39</v>
       </c>
       <c r="F35" s="126">
         <f>SUM(F3:F34)</f>
@@ -21559,13 +21801,13 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="142" t="s">
+      <c r="A37" s="164" t="s">
         <v>495</v>
       </c>
-      <c r="B37" s="142"/>
-      <c r="C37" s="142"/>
-      <c r="D37" s="142"/>
-      <c r="E37" s="142"/>
+      <c r="B37" s="164"/>
+      <c r="C37" s="164"/>
+      <c r="D37" s="164"/>
+      <c r="E37" s="164"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="120" t="s">
@@ -21652,6 +21894,76 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBA4A8B-062F-4280-B637-4D3543B7B63A}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="174" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{F954C7B2-1724-48F0-8203-4F4CA0123167}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC297CD3-0B1F-4BB7-8CC6-619A9FF0CD07}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -21672,14 +21984,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -21721,7 +22033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FCCAF4-6438-4808-B747-7037D39019AA}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -21742,14 +22054,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -21791,7 +22103,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6538CA4A-D841-48B5-87FD-DBB4645DC6A3}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -21812,14 +22124,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -21861,7 +22173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA157C68-6EB3-4779-91CE-4005608DD947}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -21882,14 +22194,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -21931,7 +22243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27645D63-80B6-4CC9-9DF9-3EC673CAFE41}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -21952,14 +22264,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22001,7 +22313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9B2914-37AB-487B-B6E7-416C38CF27C7}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -22022,14 +22334,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22071,7 +22383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148D65EB-A89E-42AB-9829-0D129960DFD3}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -22092,14 +22404,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22141,7 +22453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC9DC54-2F87-41CA-B048-C3AF3C22C7C1}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -22162,14 +22474,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22211,7 +22523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371B9012-BBC9-4C0D-A9EB-8BF65ACEAE9A}">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -22233,12 +22545,12 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="153" t="s">
+      <c r="B1" s="175" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
     </row>
@@ -22265,11 +22577,11 @@
       <c r="A3" s="32">
         <v>1</v>
       </c>
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="176" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
       <c r="E3" s="41" t="s">
         <v>150</v>
       </c>
@@ -22540,7 +22852,307 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA3E4C7-F8D1-49C5-B894-4805FFE3E511}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="39" style="149" customWidth="1"/>
+    <col min="3" max="3" width="67.140625" style="161" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="91"/>
+      <c r="B1" s="166" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="168"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="92"/>
+      <c r="B2" s="169" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="148" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="94" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="153">
+        <v>0</v>
+      </c>
+      <c r="B4" s="152" t="s">
+        <v>518</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="154"/>
+      <c r="E4" s="154"/>
+      <c r="F4" s="154"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="153"/>
+      <c r="B5" s="156" t="s">
+        <v>519</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>517</v>
+      </c>
+      <c r="D5" s="142"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="153"/>
+      <c r="B6" s="156" t="s">
+        <v>520</v>
+      </c>
+      <c r="C6" s="160" t="s">
+        <v>521</v>
+      </c>
+      <c r="D6" s="142"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="153"/>
+      <c r="B7" s="163" t="s">
+        <v>522</v>
+      </c>
+      <c r="C7" s="157" t="s">
+        <v>523</v>
+      </c>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="131"/>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="158">
+        <v>1</v>
+      </c>
+      <c r="B8" s="157" t="s">
+        <v>505</v>
+      </c>
+      <c r="C8" s="147" t="s">
+        <v>506</v>
+      </c>
+      <c r="D8" s="159"/>
+      <c r="E8" s="155"/>
+      <c r="F8" s="155"/>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="72">
+        <v>2</v>
+      </c>
+      <c r="B9" s="146" t="s">
+        <v>503</v>
+      </c>
+      <c r="C9" s="143" t="s">
+        <v>504</v>
+      </c>
+      <c r="D9" s="142"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="131"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="90">
+        <v>3</v>
+      </c>
+      <c r="B10" s="146" t="s">
+        <v>501</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>502</v>
+      </c>
+      <c r="D10" s="142"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="131"/>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="60">
+        <v>4</v>
+      </c>
+      <c r="B11" s="146" t="s">
+        <v>507</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D11" s="144"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="131"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="60">
+        <v>5</v>
+      </c>
+      <c r="B12" s="146" t="s">
+        <v>509</v>
+      </c>
+      <c r="C12" s="80" t="s">
+        <v>510</v>
+      </c>
+      <c r="D12" s="144"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="60">
+        <v>6</v>
+      </c>
+      <c r="B13" s="146" t="s">
+        <v>511</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="D13" s="144"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="145"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="60"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="145"/>
+      <c r="F14" s="145"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="63">
+        <v>7</v>
+      </c>
+      <c r="B15" s="146" t="s">
+        <v>513</v>
+      </c>
+      <c r="C15" s="80" t="s">
+        <v>514</v>
+      </c>
+      <c r="D15" s="144"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="145"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="63"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="145"/>
+      <c r="F16" s="145"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="60">
+        <v>8</v>
+      </c>
+      <c r="B17" s="146" t="s">
+        <v>515</v>
+      </c>
+      <c r="C17" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D17" s="144"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="145"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="63"/>
+      <c r="B18" s="146"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="144"/>
+      <c r="E18" s="145"/>
+      <c r="F18" s="145"/>
+    </row>
+    <row r="19" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="A19" s="63">
+        <v>9</v>
+      </c>
+      <c r="B19" s="146" t="s">
+        <v>524</v>
+      </c>
+      <c r="C19" s="80" t="s">
+        <v>525</v>
+      </c>
+      <c r="D19" s="144"/>
+      <c r="E19" s="145"/>
+      <c r="F19" s="145"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="56"/>
+      <c r="B20" s="150"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="57"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="151" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" s="162" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:F19" xr:uid="{D1AE8F92-0427-4F12-8484-D03DDDD5BCBC}"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C22" r:id="rId1" xr:uid="{6A79D70D-D845-41FE-9E25-6167BAB1DB44}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{B2EC9216-B263-4AC1-9FF3-7E2BF3C2C376}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{A3E34687-C4A2-463E-8721-3669800BEC31}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{F63BF040-4FF6-4F43-8803-ABF16117B7B2}"/>
+    <hyperlink ref="C11" r:id="rId5" xr:uid="{DDF9F7C4-6383-4E7D-A768-0B03C8ACBD51}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{DA7007F0-139E-4B22-95C5-2E9F09F21B6B}"/>
+    <hyperlink ref="C13" r:id="rId7" xr:uid="{30BD288B-6305-419D-96DA-60CDB78CE1B8}"/>
+    <hyperlink ref="C15" r:id="rId8" xr:uid="{F075282E-C1A7-4826-9ED3-93FC04F26541}"/>
+    <hyperlink ref="C17" r:id="rId9" xr:uid="{6B668F0C-C7A4-45B3-A5A8-F7C9C4887312}"/>
+    <hyperlink ref="C5" r:id="rId10" xr:uid="{F86683F4-2EDB-496D-ADB3-B8425911C417}"/>
+    <hyperlink ref="C6" r:id="rId11" location="/" xr:uid="{F6F4CB08-50FD-4ED3-87EA-A4F719F2A18C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A0C1A6-B2EA-4EC5-8484-E684C8F3E18B}">
   <dimension ref="A1:G25"/>
   <sheetViews>
@@ -22565,12 +23177,12 @@
       <c r="A1" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="156" t="s">
+      <c r="B1" s="178" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
       <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -22596,11 +23208,11 @@
       <c r="A3" s="49">
         <v>1</v>
       </c>
-      <c r="B3" s="155" t="s">
+      <c r="B3" s="177" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
       <c r="E3" s="50" t="s">
         <v>151</v>
       </c>
@@ -22677,11 +23289,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="155" t="s">
+      <c r="B12" s="177" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="155"/>
-      <c r="D12" s="155"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="177"/>
       <c r="E12" s="50" t="s">
         <v>151</v>
       </c>
@@ -22810,7 +23422,67 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E0624A-E488-4F43-A83F-9652CAB5AAD3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C00811-F6B3-4257-85C9-1B55DCD46308}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3239CF-6342-4294-A04F-B9BB3AB32E10}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCADFB6-2B39-4345-B261-07B732A46DA7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DD9AF8-082C-4A8A-B3AE-AF46DCC68640}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -22836,23 +23508,23 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="91"/>
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="166" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="148"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="168"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="92"/>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="169" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="93" t="s">
@@ -22918,7 +23590,7 @@
         <v>499</v>
       </c>
       <c r="C6" s="77"/>
-      <c r="D6" s="145" t="s">
+      <c r="D6" s="171" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="66"/>
@@ -22934,7 +23606,7 @@
       <c r="C7" s="77" t="s">
         <v>207</v>
       </c>
-      <c r="D7" s="145"/>
+      <c r="D7" s="171"/>
       <c r="E7" s="95" t="s">
         <v>498</v>
       </c>
@@ -22952,7 +23624,7 @@
       <c r="C8" s="77" t="s">
         <v>208</v>
       </c>
-      <c r="D8" s="145"/>
+      <c r="D8" s="171"/>
       <c r="E8" s="66"/>
       <c r="F8" s="66"/>
     </row>
@@ -22966,7 +23638,7 @@
       <c r="C9" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="D9" s="145"/>
+      <c r="D9" s="171"/>
       <c r="E9" s="66"/>
       <c r="F9" s="66"/>
     </row>
@@ -22980,7 +23652,7 @@
       <c r="C10" s="77" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="145"/>
+      <c r="D10" s="171"/>
       <c r="E10" s="66"/>
       <c r="F10" s="66"/>
     </row>
@@ -23177,14 +23849,14 @@
       <c r="F22" s="76"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="144" t="s">
+      <c r="A24" s="170" t="s">
         <v>219</v>
       </c>
-      <c r="B24" s="144"/>
-      <c r="C24" s="144"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="144"/>
+      <c r="B24" s="170"/>
+      <c r="C24" s="170"/>
+      <c r="D24" s="170"/>
+      <c r="E24" s="170"/>
+      <c r="F24" s="170"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="67">
@@ -23294,67 +23966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E0624A-E488-4F43-A83F-9652CAB5AAD3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C00811-F6B3-4257-85C9-1B55DCD46308}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3239CF-6342-4294-A04F-B9BB3AB32E10}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCADFB6-2B39-4345-B261-07B732A46DA7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DB7C02-07A8-4D5B-B7A9-996091B89DD9}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -23378,28 +23990,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="172" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="173" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="173"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -23692,16 +24304,16 @@
       <c r="D23" s="25"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="151" t="s">
+      <c r="A24" s="173" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="151"/>
-      <c r="C24" s="151"/>
-      <c r="D24" s="151"/>
-      <c r="E24" s="151"/>
-      <c r="F24" s="151"/>
-      <c r="G24" s="151"/>
-      <c r="H24" s="151"/>
+      <c r="B24" s="173"/>
+      <c r="C24" s="173"/>
+      <c r="D24" s="173"/>
+      <c r="E24" s="173"/>
+      <c r="F24" s="173"/>
+      <c r="G24" s="173"/>
+      <c r="H24" s="173"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
@@ -23809,7 +24421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4382FB-CCDB-4DE4-9683-3A8D07D3F404}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -23833,10 +24445,10 @@
       <c r="A1" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="152"/>
+      <c r="C1" s="174"/>
       <c r="D1" s="96"/>
       <c r="E1" s="101"/>
     </row>
@@ -23958,7 +24570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA30601C-745F-4897-9A38-C5CE8E1BD080}">
   <dimension ref="A1:A689"/>
   <sheetViews>
@@ -26943,7 +27555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8600B75A-1ED1-437D-9B1E-4EB6353449BE}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -26961,14 +27573,14 @@
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -27010,7 +27622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA77D0AC-A7B6-4319-A90C-CAC41021F832}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -27033,14 +27645,14 @@
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -27082,7 +27694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F09BD98-79D8-450C-972D-16EC9C4FC717}">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -27103,13 +27715,13 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="174" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
       <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:8" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -27225,76 +27837,6 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{0D462134-28E1-458D-AA3F-67BF5D8350E8}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBA4A8B-062F-4280-B637-4D3543B7B63A}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="152" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{F954C7B2-1724-48F0-8203-4F4CA0123167}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Durgesh Work: Timesheet updated
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Trainings\0_Training_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC3F2A7-C8CA-4D83-8CA3-33748E36B6B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3751DC6D-EE87-4A56-8B91-AFBA29611400}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="933" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
@@ -41,7 +41,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Career PATH'!$A$3:$H$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Career PATH_Improved'!$A$3:$F$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Career PATH_Interactive'!$A$3:$F$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Career PATH_Interactive'!$A$3:$F$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="531">
   <si>
     <t>SR#</t>
   </si>
@@ -8241,6 +8241,15 @@
   </si>
   <si>
     <t>7.05am - 9.05am</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/unit-testing-angular/table-of-contents</t>
+  </si>
+  <si>
+    <t>Unit Testing in Angular</t>
+  </si>
+  <si>
+    <t>7.30am - 9.53am</t>
   </si>
 </sst>
 </file>
@@ -8688,7 +8697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -9147,6 +9156,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -21168,8 +21186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4973E51C-FF21-4EFD-BEE8-1E89830C0A93}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21183,14 +21201,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="167" t="s">
         <v>494</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
-      <c r="F1" s="164"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="120" t="s">
@@ -21598,6 +21616,12 @@
       <c r="C22" s="119">
         <v>44560</v>
       </c>
+      <c r="D22" t="s">
+        <v>530</v>
+      </c>
+      <c r="E22" s="5">
+        <v>2.23</v>
+      </c>
       <c r="F22" s="5">
         <v>2</v>
       </c>
@@ -21787,13 +21811,13 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="165" t="s">
+      <c r="C35" s="168" t="s">
         <v>491</v>
       </c>
-      <c r="D35" s="165"/>
+      <c r="D35" s="168"/>
       <c r="E35" s="126">
         <f>SUM(E3:E34)</f>
-        <v>31.39</v>
+        <v>33.619999999999997</v>
       </c>
       <c r="F35" s="126">
         <f>SUM(F3:F34)</f>
@@ -21801,13 +21825,13 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="164" t="s">
+      <c r="A37" s="167" t="s">
         <v>495</v>
       </c>
-      <c r="B37" s="164"/>
-      <c r="C37" s="164"/>
-      <c r="D37" s="164"/>
-      <c r="E37" s="164"/>
+      <c r="B37" s="167"/>
+      <c r="C37" s="167"/>
+      <c r="D37" s="167"/>
+      <c r="E37" s="167"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="120" t="s">
@@ -21914,14 +21938,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -21984,14 +22008,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22054,14 +22078,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22124,14 +22148,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22194,14 +22218,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22264,14 +22288,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22334,14 +22358,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22404,14 +22428,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22474,14 +22498,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22545,12 +22569,12 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
     </row>
@@ -22577,11 +22601,11 @@
       <c r="A3" s="32">
         <v>1</v>
       </c>
-      <c r="B3" s="176" t="s">
+      <c r="B3" s="179" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
       <c r="E3" s="41" t="s">
         <v>150</v>
       </c>
@@ -22857,13 +22881,13 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22878,23 +22902,23 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="91"/>
-      <c r="B1" s="166" t="s">
+      <c r="B1" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="168"/>
+      <c r="C1" s="170"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="171"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="92"/>
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="172" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="93" t="s">
@@ -22916,37 +22940,37 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="153">
-        <v>0</v>
-      </c>
-      <c r="B4" s="152" t="s">
-        <v>518</v>
-      </c>
-      <c r="C4" s="22"/>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="164"/>
+      <c r="B4" s="166" t="s">
+        <v>529</v>
+      </c>
+      <c r="C4" s="165" t="s">
+        <v>528</v>
+      </c>
       <c r="D4" s="154"/>
       <c r="E4" s="154"/>
       <c r="F4" s="154"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="153"/>
-      <c r="B5" s="156" t="s">
-        <v>519</v>
-      </c>
-      <c r="C5" s="80" t="s">
-        <v>517</v>
-      </c>
-      <c r="D5" s="142"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
+      <c r="A5" s="153">
+        <v>0</v>
+      </c>
+      <c r="B5" s="152" t="s">
+        <v>518</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="154"/>
+      <c r="E5" s="154"/>
+      <c r="F5" s="154"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="153"/>
       <c r="B6" s="156" t="s">
-        <v>520</v>
-      </c>
-      <c r="C6" s="160" t="s">
-        <v>521</v>
+        <v>519</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>517</v>
       </c>
       <c r="D6" s="142"/>
       <c r="E6" s="131"/>
@@ -22954,201 +22978,214 @@
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="153"/>
-      <c r="B7" s="163" t="s">
+      <c r="B7" s="156" t="s">
+        <v>520</v>
+      </c>
+      <c r="C7" s="160" t="s">
+        <v>521</v>
+      </c>
+      <c r="D7" s="142"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="131"/>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="153"/>
+      <c r="B8" s="163" t="s">
         <v>522</v>
       </c>
-      <c r="C7" s="157" t="s">
+      <c r="C8" s="157" t="s">
         <v>523</v>
       </c>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="131"/>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="158">
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="131"/>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="158">
         <v>1</v>
       </c>
-      <c r="B8" s="157" t="s">
+      <c r="B9" s="157" t="s">
         <v>505</v>
       </c>
-      <c r="C8" s="147" t="s">
+      <c r="C9" s="147" t="s">
         <v>506</v>
       </c>
-      <c r="D8" s="159"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="155"/>
-    </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="72">
+      <c r="D9" s="159"/>
+      <c r="E9" s="155"/>
+      <c r="F9" s="155"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="72">
         <v>2</v>
       </c>
-      <c r="B9" s="146" t="s">
+      <c r="B10" s="146" t="s">
         <v>503</v>
       </c>
-      <c r="C9" s="143" t="s">
+      <c r="C10" s="143" t="s">
         <v>504</v>
-      </c>
-      <c r="D9" s="142"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
-    </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="90">
-        <v>3</v>
-      </c>
-      <c r="B10" s="146" t="s">
-        <v>501</v>
-      </c>
-      <c r="C10" s="80" t="s">
-        <v>502</v>
       </c>
       <c r="D10" s="142"/>
       <c r="E10" s="131"/>
       <c r="F10" s="131"/>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="60">
-        <v>4</v>
+      <c r="A11" s="90">
+        <v>3</v>
       </c>
       <c r="B11" s="146" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="C11" s="80" t="s">
-        <v>508</v>
-      </c>
-      <c r="D11" s="144"/>
+        <v>502</v>
+      </c>
+      <c r="D11" s="142"/>
       <c r="E11" s="131"/>
       <c r="F11" s="131"/>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="146" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C12" s="80" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D12" s="144"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="145"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="60">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C13" s="80" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D13" s="144"/>
       <c r="E13" s="145"/>
       <c r="F13" s="145"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
-      <c r="B14" s="146"/>
-      <c r="C14" s="80"/>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="60">
+        <v>6</v>
+      </c>
+      <c r="B14" s="146" t="s">
+        <v>511</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>512</v>
+      </c>
       <c r="D14" s="144"/>
       <c r="E14" s="145"/>
       <c r="F14" s="145"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="63">
-        <v>7</v>
-      </c>
-      <c r="B15" s="146" t="s">
-        <v>513</v>
-      </c>
-      <c r="C15" s="80" t="s">
-        <v>514</v>
-      </c>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="60"/>
+      <c r="B15" s="146"/>
+      <c r="C15" s="80"/>
       <c r="D15" s="144"/>
       <c r="E15" s="145"/>
       <c r="F15" s="145"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="63"/>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="63">
+        <v>7</v>
+      </c>
+      <c r="B16" s="146" t="s">
+        <v>513</v>
+      </c>
+      <c r="C16" s="80" t="s">
+        <v>514</v>
+      </c>
       <c r="D16" s="144"/>
       <c r="E16" s="145"/>
       <c r="F16" s="145"/>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="60">
-        <v>8</v>
-      </c>
-      <c r="B17" s="146" t="s">
-        <v>515</v>
-      </c>
-      <c r="C17" s="80" t="s">
-        <v>516</v>
-      </c>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="63"/>
       <c r="D17" s="144"/>
       <c r="E17" s="145"/>
       <c r="F17" s="145"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="63"/>
-      <c r="B18" s="146"/>
-      <c r="C18" s="81"/>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="60">
+        <v>8</v>
+      </c>
+      <c r="B18" s="146" t="s">
+        <v>515</v>
+      </c>
+      <c r="C18" s="80" t="s">
+        <v>516</v>
+      </c>
       <c r="D18" s="144"/>
       <c r="E18" s="145"/>
       <c r="F18" s="145"/>
     </row>
-    <row r="19" spans="1:6" ht="210" x14ac:dyDescent="0.25">
-      <c r="A19" s="63">
-        <v>9</v>
-      </c>
-      <c r="B19" s="146" t="s">
-        <v>524</v>
-      </c>
-      <c r="C19" s="80" t="s">
-        <v>525</v>
-      </c>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="63"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="81"/>
       <c r="D19" s="144"/>
       <c r="E19" s="145"/>
       <c r="F19" s="145"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
-      <c r="B20" s="150"/>
-      <c r="D20" s="1"/>
+    <row r="20" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="A20" s="63">
+        <v>9</v>
+      </c>
+      <c r="B20" s="146" t="s">
+        <v>524</v>
+      </c>
+      <c r="C20" s="80" t="s">
+        <v>525</v>
+      </c>
+      <c r="D20" s="144"/>
+      <c r="E20" s="145"/>
+      <c r="F20" s="145"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="57"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="150"/>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="151" t="s">
+      <c r="A22" s="57"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="151" t="s">
         <v>218</v>
       </c>
-      <c r="C22" s="162" t="s">
+      <c r="C23" s="162" t="s">
         <v>216</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F19" xr:uid="{D1AE8F92-0427-4F12-8484-D03DDDD5BCBC}"/>
+  <autoFilter ref="A3:F20" xr:uid="{D1AE8F92-0427-4F12-8484-D03DDDD5BCBC}"/>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C22" r:id="rId1" xr:uid="{6A79D70D-D845-41FE-9E25-6167BAB1DB44}"/>
-    <hyperlink ref="C10" r:id="rId2" xr:uid="{B2EC9216-B263-4AC1-9FF3-7E2BF3C2C376}"/>
-    <hyperlink ref="C9" r:id="rId3" xr:uid="{A3E34687-C4A2-463E-8721-3669800BEC31}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{F63BF040-4FF6-4F43-8803-ABF16117B7B2}"/>
-    <hyperlink ref="C11" r:id="rId5" xr:uid="{DDF9F7C4-6383-4E7D-A768-0B03C8ACBD51}"/>
-    <hyperlink ref="C12" r:id="rId6" xr:uid="{DA7007F0-139E-4B22-95C5-2E9F09F21B6B}"/>
-    <hyperlink ref="C13" r:id="rId7" xr:uid="{30BD288B-6305-419D-96DA-60CDB78CE1B8}"/>
-    <hyperlink ref="C15" r:id="rId8" xr:uid="{F075282E-C1A7-4826-9ED3-93FC04F26541}"/>
-    <hyperlink ref="C17" r:id="rId9" xr:uid="{6B668F0C-C7A4-45B3-A5A8-F7C9C4887312}"/>
-    <hyperlink ref="C5" r:id="rId10" xr:uid="{F86683F4-2EDB-496D-ADB3-B8425911C417}"/>
-    <hyperlink ref="C6" r:id="rId11" location="/" xr:uid="{F6F4CB08-50FD-4ED3-87EA-A4F719F2A18C}"/>
+    <hyperlink ref="C23" r:id="rId1" xr:uid="{6A79D70D-D845-41FE-9E25-6167BAB1DB44}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{B2EC9216-B263-4AC1-9FF3-7E2BF3C2C376}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{A3E34687-C4A2-463E-8721-3669800BEC31}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{F63BF040-4FF6-4F43-8803-ABF16117B7B2}"/>
+    <hyperlink ref="C12" r:id="rId5" xr:uid="{DDF9F7C4-6383-4E7D-A768-0B03C8ACBD51}"/>
+    <hyperlink ref="C13" r:id="rId6" xr:uid="{DA7007F0-139E-4B22-95C5-2E9F09F21B6B}"/>
+    <hyperlink ref="C14" r:id="rId7" xr:uid="{30BD288B-6305-419D-96DA-60CDB78CE1B8}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{F075282E-C1A7-4826-9ED3-93FC04F26541}"/>
+    <hyperlink ref="C18" r:id="rId9" xr:uid="{6B668F0C-C7A4-45B3-A5A8-F7C9C4887312}"/>
+    <hyperlink ref="C6" r:id="rId10" xr:uid="{F86683F4-2EDB-496D-ADB3-B8425911C417}"/>
+    <hyperlink ref="C7" r:id="rId11" location="/" xr:uid="{F6F4CB08-50FD-4ED3-87EA-A4F719F2A18C}"/>
+    <hyperlink ref="C4" r:id="rId12" xr:uid="{25A06C2E-7FAB-426F-A49F-8BE0057C63EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -23177,12 +23214,12 @@
       <c r="A1" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="178" t="s">
+      <c r="B1" s="181" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
       <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -23208,11 +23245,11 @@
       <c r="A3" s="49">
         <v>1</v>
       </c>
-      <c r="B3" s="177" t="s">
+      <c r="B3" s="180" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="180"/>
       <c r="E3" s="50" t="s">
         <v>151</v>
       </c>
@@ -23289,11 +23326,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="177" t="s">
+      <c r="B12" s="180" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="177"/>
-      <c r="D12" s="177"/>
+      <c r="C12" s="180"/>
+      <c r="D12" s="180"/>
       <c r="E12" s="50" t="s">
         <v>151</v>
       </c>
@@ -23508,23 +23545,23 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="91"/>
-      <c r="B1" s="166" t="s">
+      <c r="B1" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="168"/>
+      <c r="C1" s="170"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="171"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="92"/>
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="172" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="93" t="s">
@@ -23590,7 +23627,7 @@
         <v>499</v>
       </c>
       <c r="C6" s="77"/>
-      <c r="D6" s="171" t="s">
+      <c r="D6" s="174" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="66"/>
@@ -23606,7 +23643,7 @@
       <c r="C7" s="77" t="s">
         <v>207</v>
       </c>
-      <c r="D7" s="171"/>
+      <c r="D7" s="174"/>
       <c r="E7" s="95" t="s">
         <v>498</v>
       </c>
@@ -23624,7 +23661,7 @@
       <c r="C8" s="77" t="s">
         <v>208</v>
       </c>
-      <c r="D8" s="171"/>
+      <c r="D8" s="174"/>
       <c r="E8" s="66"/>
       <c r="F8" s="66"/>
     </row>
@@ -23638,7 +23675,7 @@
       <c r="C9" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="D9" s="171"/>
+      <c r="D9" s="174"/>
       <c r="E9" s="66"/>
       <c r="F9" s="66"/>
     </row>
@@ -23652,7 +23689,7 @@
       <c r="C10" s="77" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="171"/>
+      <c r="D10" s="174"/>
       <c r="E10" s="66"/>
       <c r="F10" s="66"/>
     </row>
@@ -23849,14 +23886,14 @@
       <c r="F22" s="76"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="170" t="s">
+      <c r="A24" s="173" t="s">
         <v>219</v>
       </c>
-      <c r="B24" s="170"/>
-      <c r="C24" s="170"/>
-      <c r="D24" s="170"/>
-      <c r="E24" s="170"/>
-      <c r="F24" s="170"/>
+      <c r="B24" s="173"/>
+      <c r="C24" s="173"/>
+      <c r="D24" s="173"/>
+      <c r="E24" s="173"/>
+      <c r="F24" s="173"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="67">
@@ -23990,28 +24027,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="175" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="176" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -24304,16 +24341,16 @@
       <c r="D23" s="25"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="173" t="s">
+      <c r="A24" s="176" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="173"/>
-      <c r="C24" s="173"/>
-      <c r="D24" s="173"/>
-      <c r="E24" s="173"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="173"/>
-      <c r="H24" s="173"/>
+      <c r="B24" s="176"/>
+      <c r="C24" s="176"/>
+      <c r="D24" s="176"/>
+      <c r="E24" s="176"/>
+      <c r="F24" s="176"/>
+      <c r="G24" s="176"/>
+      <c r="H24" s="176"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
@@ -24445,10 +24482,10 @@
       <c r="A1" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="174"/>
+      <c r="C1" s="177"/>
       <c r="D1" s="96"/>
       <c r="E1" s="101"/>
     </row>
@@ -27573,14 +27610,14 @@
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -27645,14 +27682,14 @@
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -27715,13 +27752,13 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="177" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
       <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:8" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -27853,6 +27890,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024D76020AE708242B68336FA618CBCDF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d53f460e102142885dbc8938524af06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df3f84f5-0dce-435a-abac-67420900ba59" xmlns:ns4="c8965576-7528-46e3-a68d-d4bc5141fdaa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51dd3132ab51039a0b8a02bab29c14ac" ns3:_="" ns4:_="">
     <xsd:import namespace="df3f84f5-0dce-435a-abac-67420900ba59"/>
@@ -28075,12 +28118,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC37F108-450B-470C-B7B9-209E1FAF9670}">
   <ds:schemaRefs>
@@ -28090,6 +28127,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{236AB03D-89C6-4FEB-AC3B-BF68DD4F8BD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c8965576-7528-46e3-a68d-d4bc5141fdaa"/>
+    <ds:schemaRef ds:uri="df3f84f5-0dce-435a-abac-67420900ba59"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC42E61D-1BC2-43F5-95E9-ABDA8B3BC8C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28106,21 +28160,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{236AB03D-89C6-4FEB-AC3B-BF68DD4F8BD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c8965576-7528-46e3-a68d-d4bc5141fdaa"/>
-    <ds:schemaRef ds:uri="df3f84f5-0dce-435a-abac-67420900ba59"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>